<commit_message>
integrate drill into system
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9312BA92-B577-44FC-A702-73D260F447A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534390BA-A0FF-478D-8DF3-E5D93DBD41E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,7 +2958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>116</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>117</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>118</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>119</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>120</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>

</xml_diff>

<commit_message>
work on drill related mobules
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534390BA-A0FF-478D-8DF3-E5D93DBD41E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14B1A72-89E8-4FBF-9AE6-0227B65ACE90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="123">
   <si>
     <t>عنوان</t>
   </si>
@@ -383,6 +383,12 @@
   </si>
   <si>
     <t>ايجاد، حذف، نمايش و ويرايش بخش انواع نمونه‌هاي فاكتورهاي ارزيابي گروهاي سني (agelevel_metrics)</t>
+  </si>
+  <si>
+    <t>تعريف شيوه محاسبه و تعيين رده سني بازيكنان براساس استاندارد تعريف شده فدراسيون</t>
+  </si>
+  <si>
+    <t>امكان به‌روز رساني دوره اي رده سني بازيكنان براساس استاندارد تعريف شده در نرم افزار</t>
   </si>
 </sst>
 </file>
@@ -418,13 +424,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -469,8 +481,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F119" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:F119" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F121" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:F121" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
     <filterColumn colId="1">
       <filters>
         <filter val="دوم"/>
@@ -757,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F119"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3065,6 +3077,46 @@
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
     </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C120" s="4">
+        <v>0</v>
+      </c>
+      <c r="D120" s="4">
+        <v>0</v>
+      </c>
+      <c r="E120" s="4">
+        <v>0</v>
+      </c>
+      <c r="F120" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C121" s="4">
+        <v>0</v>
+      </c>
+      <c r="D121" s="4">
+        <v>0</v>
+      </c>
+      <c r="E121" s="4">
+        <v>0</v>
+      </c>
+      <c r="F121" s="4">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
coach certificate levels delivered
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0287A2BB-21CA-404C-A2F0-A89DCFD69C45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5429D9AF-1526-4531-B6C8-5704BDFC70C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -772,7 +772,7 @@
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130"/>
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,16 +2758,16 @@
         <v>31</v>
       </c>
       <c r="C103" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D103" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F103" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
club agelevel has updated
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C521637-4A10-4599-810F-F6D03175D02C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711E2EA6-2D06-4E21-B709-111A648FE286}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="124">
   <si>
     <t>عنوان</t>
   </si>
@@ -389,6 +389,9 @@
   </si>
   <si>
     <t>محاسبه زمان مناسب براي برگزاري تمرين براساس الگوي تمريني انتخاب شده (محاسبه طول تمرين براساس طول تمرين پيشنهادي در برنامه تمريني)</t>
+  </si>
+  <si>
+    <t>افزودن آيتم مربيان به بخش كلاس آموزشي</t>
   </si>
 </sst>
 </file>
@@ -481,14 +484,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F121" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:F121" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F122" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:F122" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
     <filterColumn colId="1">
       <filters>
         <filter val="دوم"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="2">
+    <filterColumn colId="5">
       <filters>
         <filter val="0"/>
       </filters>
@@ -769,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F106" sqref="F106"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,15 +1145,15 @@
         <v>1</v>
       </c>
       <c r="F18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -1382,7 +1385,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1505,12 +1508,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C37" s="1">
         <v>0</v>
@@ -1542,7 +1545,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1565,12 +1568,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C40" s="1">
         <v>0</v>
@@ -1722,7 +1725,7 @@
         <v>1</v>
       </c>
       <c r="F47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1782,7 +1785,7 @@
         <v>1</v>
       </c>
       <c r="F50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1802,7 +1805,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1822,7 +1825,7 @@
         <v>1</v>
       </c>
       <c r="F52" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1873,16 +1876,16 @@
         <v>31</v>
       </c>
       <c r="C55" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1925,12 +1928,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C58" s="1">
         <v>0</v>
@@ -1945,12 +1948,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C59" s="1">
         <v>0</v>
@@ -1965,12 +1968,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C60" s="1">
         <v>0</v>
@@ -2284,7 +2287,7 @@
         <v>79</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="C77" s="1">
         <v>0</v>
@@ -2433,12 +2436,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C86" s="1">
         <v>0</v>
@@ -2540,12 +2543,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C92" s="1">
         <v>0</v>
@@ -2680,12 +2683,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C99" s="1">
         <v>0</v>
@@ -2727,7 +2730,7 @@
         <v>1</v>
       </c>
       <c r="F101" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2770,7 +2773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>104</v>
       </c>
@@ -2890,7 +2893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>111</v>
       </c>
@@ -2898,19 +2901,19 @@
         <v>31</v>
       </c>
       <c r="C110" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D110" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F110" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>112</v>
       </c>
@@ -2918,24 +2921,24 @@
         <v>31</v>
       </c>
       <c r="C111" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D111" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E111" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F111" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C112" s="1">
         <v>0</v>
@@ -3114,6 +3117,26 @@
         <v>0</v>
       </c>
       <c r="F121" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C122" s="4">
+        <v>0</v>
+      </c>
+      <c r="D122" s="4">
+        <v>0</v>
+      </c>
+      <c r="E122" s="4">
+        <v>0</v>
+      </c>
+      <c r="F122" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
trouble on certificate levels
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711E2EA6-2D06-4E21-B709-111A648FE286}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927C11C6-70EF-4B09-82F0-6E2DBF566CEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -775,7 +775,7 @@
   <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1868,7 +1868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
work on drill patterns
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D227C9F-EBB2-48C2-8BF0-662BA0041160}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33DCBD9-10F7-4D5A-85D0-5E12CE4A88F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="127">
   <si>
     <t>عنوان</t>
   </si>
@@ -392,6 +392,15 @@
   </si>
   <si>
     <t>افزودن آيتم مربيان به بخش كلاس آموزشي</t>
+  </si>
+  <si>
+    <t>تعريف تمامي آيتم‌هاي ثابت به صورت يك متغير در كلاس‌هاي بخش Library</t>
+  </si>
+  <si>
+    <t>ايجاد، حذف، نمايش و ويرايش بخش الگوهاي برنامه ريزي تمرين</t>
+  </si>
+  <si>
+    <t>ايجاد نمايش تقويمي كلاس آموزشي براساس روزهاي تمرين و لينك به جزئيات جلسه تمرين</t>
   </si>
 </sst>
 </file>
@@ -484,8 +493,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F122" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:F122" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F126" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:F126" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
     <filterColumn colId="1">
       <filters>
         <filter val="دوم"/>
@@ -772,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F122"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,10 +1125,10 @@
         <v>31</v>
       </c>
       <c r="C17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -1168,12 +1177,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -1268,12 +1277,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
@@ -1848,12 +1857,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C54" s="1">
         <v>0</v>
@@ -3138,6 +3147,73 @@
       </c>
       <c r="F122" s="4">
         <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C123" s="4">
+        <v>0</v>
+      </c>
+      <c r="D123" s="4">
+        <v>0</v>
+      </c>
+      <c r="E123" s="4">
+        <v>0</v>
+      </c>
+      <c r="F123" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C124" s="4">
+        <v>1</v>
+      </c>
+      <c r="D124" s="4">
+        <v>1</v>
+      </c>
+      <c r="E124" s="4">
+        <v>0</v>
+      </c>
+      <c r="F124" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C126" s="4">
+        <v>0</v>
+      </c>
+      <c r="D126" s="4">
+        <v>0</v>
+      </c>
+      <c r="E126" s="4">
+        <v>0</v>
+      </c>
+      <c r="F126" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on drill pattern items
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33DCBD9-10F7-4D5A-85D0-5E12CE4A88F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F109CE03-67C0-4C9F-ACD1-E82A27170847}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="128">
   <si>
     <t>عنوان</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>ايجاد نمايش تقويمي كلاس آموزشي براساس روزهاي تمرين و لينك به جزئيات جلسه تمرين</t>
+  </si>
+  <si>
+    <t>ايجاد، حذف، نمايش و ويرايش بخش آيتم‌هاي تمريني الگوي تمرين</t>
   </si>
 </sst>
 </file>
@@ -493,8 +496,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F126" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:F126" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F128" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:F128" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
     <filterColumn colId="1">
       <filters>
         <filter val="دوم"/>
@@ -781,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F128"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+      <selection activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3169,7 +3172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>125</v>
       </c>
@@ -3183,10 +3186,10 @@
         <v>1</v>
       </c>
       <c r="E124" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F124" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -3196,7 +3199,7 @@
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>126</v>
       </c>
@@ -3213,6 +3216,33 @@
         <v>0</v>
       </c>
       <c r="F126" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="4"/>
+      <c r="C127" s="4"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="4"/>
+      <c r="F127" s="4"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C128" s="4">
+        <v>1</v>
+      </c>
+      <c r="D128" s="4">
+        <v>1</v>
+      </c>
+      <c r="E128" s="4">
+        <v>0</v>
+      </c>
+      <c r="F128" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
testing drill pattern items
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F109CE03-67C0-4C9F-ACD1-E82A27170847}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF310682-6B80-4574-A6E0-A2A00735A5C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="129">
   <si>
     <t>عنوان</t>
   </si>
@@ -404,6 +404,9 @@
   </si>
   <si>
     <t>ايجاد، حذف، نمايش و ويرايش بخش آيتم‌هاي تمريني الگوي تمرين</t>
+  </si>
+  <si>
+    <t>ايجاد پيش نمايش براي هر الگوي تمرين به صورت هفتگي</t>
   </si>
 </sst>
 </file>
@@ -496,8 +499,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F128" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:F128" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F129" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:F129" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
     <filterColumn colId="1">
       <filters>
         <filter val="دوم"/>
@@ -784,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F128"/>
+  <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F106" sqref="F106"/>
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3240,9 +3243,29 @@
         <v>1</v>
       </c>
       <c r="E128" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F128" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C129" s="4">
+        <v>0</v>
+      </c>
+      <c r="D129" s="4">
+        <v>0</v>
+      </c>
+      <c r="E129" s="4">
+        <v>0</v>
+      </c>
+      <c r="F129" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finilize weekly simulation of pattern items
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF310682-6B80-4574-A6E0-A2A00735A5C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7252A8-FB20-413D-B4C7-D7B60BB3797B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="130">
   <si>
     <t>عنوان</t>
   </si>
@@ -407,6 +407,9 @@
   </si>
   <si>
     <t>ايجاد پيش نمايش براي هر الگوي تمرين به صورت هفتگي</t>
+  </si>
+  <si>
+    <t>ايجاد داشبورد نمايشي برنامه هفتگي تمرينات دوره آموزشي</t>
   </si>
 </sst>
 </file>
@@ -499,8 +502,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F129" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:F129" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F130" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:F130" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
     <filterColumn colId="1">
       <filters>
         <filter val="دوم"/>
@@ -787,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3229,7 +3232,7 @@
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>127</v>
       </c>
@@ -3246,10 +3249,10 @@
         <v>1</v>
       </c>
       <c r="F128" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>128</v>
       </c>
@@ -3257,15 +3260,35 @@
         <v>31</v>
       </c>
       <c r="C129" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D129" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E129" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F129" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C130" s="4">
+        <v>0</v>
+      </c>
+      <c r="D130" s="4">
+        <v>0</v>
+      </c>
+      <c r="E130" s="4">
+        <v>0</v>
+      </c>
+      <c r="F130" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
delivery on 31 jan 2021
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7252A8-FB20-413D-B4C7-D7B60BB3797B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E160A8B2-FC0D-49A2-BBAE-51ACB3A805AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="131">
   <si>
     <t>عنوان</t>
   </si>
@@ -410,6 +410,9 @@
   </si>
   <si>
     <t>ايجاد داشبورد نمايشي برنامه هفتگي تمرينات دوره آموزشي</t>
+  </si>
+  <si>
+    <t>تغيير نام كنترلر club به training_class</t>
   </si>
 </sst>
 </file>
@@ -502,8 +505,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F130" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:F130" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F131" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:F131" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
     <filterColumn colId="1">
       <filters>
         <filter val="دوم"/>
@@ -790,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F130"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+      <selection activeCell="F131" sqref="F131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,10 +1857,10 @@
         <v>31</v>
       </c>
       <c r="C53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -3280,7 +3283,7 @@
         <v>31</v>
       </c>
       <c r="C130" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D130" s="4">
         <v>0</v>
@@ -3289,6 +3292,26 @@
         <v>0</v>
       </c>
       <c r="F130" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C131" s="4">
+        <v>0</v>
+      </c>
+      <c r="D131" s="4">
+        <v>0</v>
+      </c>
+      <c r="E131" s="4">
+        <v>0</v>
+      </c>
+      <c r="F131" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
work on training preview UI
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05CC16D-64C7-4A96-A967-D4BC2B9BE255}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7750B69-1A7E-4DCA-B1A6-79D430FA3933}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="134">
   <si>
     <t>عنوان</t>
   </si>
@@ -416,6 +416,12 @@
   </si>
   <si>
     <t>ايجاد، حذف، نمايش و ويرايش بخش قالب‌هاي تمريني فصلي(PlanTemplate)</t>
+  </si>
+  <si>
+    <t>افزودن بخش تنظيمات مربوط به تاريخ (تاريخ پايه اي سيستم، روز اول هفته، روزهاي تعطيل رسمي و ...)</t>
+  </si>
+  <si>
+    <t>افزودن بخش</t>
   </si>
 </sst>
 </file>
@@ -508,8 +514,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F133" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:F133" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F136" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:F136" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
     <filterColumn colId="1">
       <filters>
         <filter val="دوم"/>
@@ -796,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+      <selection activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,7 +1858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>121</v>
       </c>
@@ -1866,10 +1872,10 @@
         <v>1</v>
       </c>
       <c r="E53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -3344,6 +3350,43 @@
       <c r="F133" s="4">
         <v>0</v>
       </c>
+    </row>
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C134" s="4">
+        <v>0</v>
+      </c>
+      <c r="D134" s="4">
+        <v>0</v>
+      </c>
+      <c r="E134" s="4">
+        <v>0</v>
+      </c>
+      <c r="F134" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B135" s="4"/>
+      <c r="C135" s="4"/>
+      <c r="D135" s="4"/>
+      <c r="E135" s="4"/>
+      <c r="F135" s="4"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B136" s="4"/>
+      <c r="C136" s="4"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="4"/>
+      <c r="F136" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
some issue on showing drills
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7750B69-1A7E-4DCA-B1A6-79D430FA3933}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E620F5DA-8FC5-4425-89C3-FBBFE6386AF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -805,7 +805,7 @@
   <dimension ref="A1:F136"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3295,10 +3295,10 @@
         <v>1</v>
       </c>
       <c r="D130" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E130" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F130" s="4">
         <v>0</v>
@@ -3331,15 +3331,15 @@
       <c r="E132" s="4"/>
       <c r="F132" s="4"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C133" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D133" s="4">
         <v>0</v>
@@ -3381,7 +3381,7 @@
       <c r="E135" s="4"/>
       <c r="F135" s="4"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
       <c r="D136" s="4"/>

</xml_diff>

<commit_message>
training calendar view has delivered
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E620F5DA-8FC5-4425-89C3-FBBFE6386AF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DD4F72-0680-4DF8-A924-8C6C92F6E83D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="136">
   <si>
     <t>عنوان</t>
   </si>
@@ -422,6 +422,12 @@
   </si>
   <si>
     <t>افزودن بخش</t>
+  </si>
+  <si>
+    <t>افزودن قابليت صفحه بندي به ليست هاي موجود در نرم افزار</t>
+  </si>
+  <si>
+    <t>قابليت ورود به نرم افزار و افزودن سطح دسترسي به بخش هاي مختلف</t>
   </si>
 </sst>
 </file>
@@ -514,8 +520,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F136" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:F136" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F138" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:F138" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
     <filterColumn colId="1">
       <filters>
         <filter val="دوم"/>
@@ -802,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+      <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3301,7 +3307,7 @@
         <v>1</v>
       </c>
       <c r="F130" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -3387,6 +3393,46 @@
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
       <c r="F136" s="4"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C137" s="4">
+        <v>0</v>
+      </c>
+      <c r="D137" s="4">
+        <v>0</v>
+      </c>
+      <c r="E137" s="4">
+        <v>0</v>
+      </c>
+      <c r="F137" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C138" s="4">
+        <v>0</v>
+      </c>
+      <c r="D138" s="4">
+        <v>0</v>
+      </c>
+      <c r="E138" s="4">
+        <v>0</v>
+      </c>
+      <c r="F138" s="4">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
data synced + controller added
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DD4F72-0680-4DF8-A924-8C6C92F6E83D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB856D27-C481-4F02-8F58-EF9667CE2A94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -811,7 +811,7 @@
   <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98"/>
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,10 +1952,10 @@
         <v>31</v>
       </c>
       <c r="C57" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -3290,7 +3290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>129</v>
       </c>
@@ -3422,10 +3422,10 @@
         <v>31</v>
       </c>
       <c r="C138" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D138" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E138" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
plan update 8 feb 2021
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB856D27-C481-4F02-8F58-EF9667CE2A94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307D4825-2527-4B7E-99BD-330985A338AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -811,7 +811,7 @@
   <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
work on zones and components
</commit_message>
<xml_diff>
--- a/planning/backlog(AutoRecovered).xlsx
+++ b/planning/backlog(AutoRecovered).xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DF2CF5-66EF-40ED-B718-791878DDAE09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A43B80D-076F-4585-AD84-66F022BF1097}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="147">
   <si>
     <t>عنوان</t>
   </si>
@@ -455,6 +456,12 @@
   </si>
   <si>
     <t>ايجاد، حذف، نمايش و ويرايش كاربران گروه</t>
+  </si>
+  <si>
+    <t>ايجاد، حذف، نمايش و ويرايش بخش zone هاي دسترسي كاربران</t>
+  </si>
+  <si>
+    <t>ايجاد، حذف، نمايش و ويرايش بخش componentهاي نرم افزار</t>
   </si>
 </sst>
 </file>
@@ -547,8 +554,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F148" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:F148" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E469938-03BB-46A3-9857-9EF05EB325D4}" name="Table1" displayName="Table1" ref="A1:F151" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:F151" xr:uid="{9220B664-2E3C-4A3D-AEBB-11C047D8DB45}">
     <filterColumn colId="1">
       <filters>
         <filter val="دوم"/>
@@ -835,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E155" sqref="E155"/>
+      <selection activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>66</v>
       </c>
@@ -3647,6 +3654,53 @@
       <c r="F148" s="4">
         <v>1</v>
       </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C149" s="4">
+        <v>0</v>
+      </c>
+      <c r="D149" s="4">
+        <v>0</v>
+      </c>
+      <c r="E149" s="4">
+        <v>0</v>
+      </c>
+      <c r="F149" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C150" s="4">
+        <v>0</v>
+      </c>
+      <c r="D150" s="4">
+        <v>0</v>
+      </c>
+      <c r="E150" s="4">
+        <v>0</v>
+      </c>
+      <c r="F150" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B151" s="4"/>
+      <c r="C151" s="4"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="4"/>
+      <c r="F151" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>